<commit_message>
Fix table importing and printing
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3jerr\Documents\School\3A BME\CS360 Intro to Database\Term Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E08BBB3D-4B67-4655-932E-8B1370FEAEB7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157BCFFE-2140-4924-85FA-25F7C7E7E588}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{35BB2C26-138C-4991-94DE-4A53C5FD6E8A}"/>
   </bookViews>
@@ -380,7 +380,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>